<commit_message>
0110 tony consume and rfidinput
</commit_message>
<xml_diff>
--- a/public/download/ConsumeExample.xlsx
+++ b/public/download/ConsumeExample.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t xml:space="preserve">客戶別</t>
   </si>
@@ -35,6 +35,18 @@
   </si>
   <si>
     <t xml:space="preserve">單耗</t>
+  </si>
+  <si>
+    <t xml:space="preserve">當月MPS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">當月生產天數</t>
+  </si>
+  <si>
+    <t xml:space="preserve">下月MPS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">下月生產天數</t>
   </si>
   <si>
     <t xml:space="preserve">Fendi</t>
@@ -149,10 +161,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J16" activeCellId="0" sqref="J16"/>
+      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -177,22 +189,46 @@
       <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>10</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>